<commit_message>
Different import optoins etc.
</commit_message>
<xml_diff>
--- a/Benchmarking/Clean_Oneill_SCSSCalc_July2020.xlsx
+++ b/Benchmarking/Clean_Oneill_SCSSCalc_July2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PySulfSat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\Benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1DC616-F378-4E2B-8F87-E176105A567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F140C118-DD72-4D27-B2E0-86338510417F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCSS Calculator" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="FeOt vs. S" sheetId="4" r:id="rId3"/>
     <sheet name="Python_Input" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1497,6 +1497,51 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="8" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1577,51 +1622,6 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="8" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -5643,36 +5643,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY207"/>
   <sheetViews>
-    <sheetView topLeftCell="J23" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14:U49"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.796875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="13" max="14" width="10.796875" style="1"/>
-    <col min="15" max="16" width="11.69921875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="3.19921875" style="2" customWidth="1"/>
-    <col min="18" max="19" width="13.296875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="3.296875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="13.19921875" style="122" customWidth="1"/>
-    <col min="22" max="23" width="10.796875" style="2"/>
-    <col min="24" max="24" width="3.296875" customWidth="1"/>
+    <col min="13" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="16" width="11.6640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="3.1640625" style="2" customWidth="1"/>
+    <col min="18" max="19" width="13.33203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="3.33203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" style="95" customWidth="1"/>
+    <col min="22" max="23" width="10.83203125" style="2"/>
+    <col min="24" max="24" width="3.33203125" customWidth="1"/>
     <col min="35" max="35" width="3" customWidth="1"/>
-    <col min="36" max="36" width="13.296875" style="3" customWidth="1"/>
-    <col min="37" max="37" width="13.296875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="13.296875" style="3" customWidth="1"/>
-    <col min="39" max="39" width="3.19921875" customWidth="1"/>
-    <col min="40" max="40" width="12.19921875" style="3" customWidth="1"/>
-    <col min="41" max="41" width="11.69921875" style="3" customWidth="1"/>
-    <col min="42" max="42" width="10.796875" style="3"/>
-    <col min="43" max="43" width="10.796875" style="3" customWidth="1"/>
+    <col min="36" max="36" width="13.33203125" style="3" customWidth="1"/>
+    <col min="37" max="37" width="13.33203125" style="1" customWidth="1"/>
+    <col min="38" max="38" width="13.33203125" style="3" customWidth="1"/>
+    <col min="39" max="39" width="3.1640625" customWidth="1"/>
+    <col min="40" max="40" width="12.1640625" style="3" customWidth="1"/>
+    <col min="41" max="41" width="11.6640625" style="3" customWidth="1"/>
+    <col min="42" max="42" width="10.83203125" style="3"/>
+    <col min="43" max="43" width="10.83203125" style="3" customWidth="1"/>
     <col min="44" max="44" width="15" style="3" customWidth="1"/>
-    <col min="45" max="45" width="3.19921875" customWidth="1"/>
-    <col min="46" max="51" width="10.796875" style="3"/>
+    <col min="45" max="45" width="3.1640625" customWidth="1"/>
+    <col min="46" max="51" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51">
@@ -5681,11 +5681,11 @@
       </c>
     </row>
     <row r="3" spans="1:51">
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="103"/>
       <c r="F3" s="66"/>
       <c r="G3" s="66"/>
       <c r="H3" s="66"/>
@@ -5699,18 +5699,18 @@
       <c r="P3" s="66"/>
     </row>
     <row r="4" spans="1:51">
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
     </row>
     <row r="5" spans="1:51">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="92"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -5722,12 +5722,12 @@
       <c r="AX5"/>
       <c r="AY5"/>
     </row>
-    <row r="6" spans="1:51" ht="16.05" customHeight="1">
-      <c r="B6" s="93" t="s">
+    <row r="6" spans="1:51" ht="16" customHeight="1">
+      <c r="B6" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="112"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -5740,9 +5740,9 @@
       <c r="AY6"/>
     </row>
     <row r="7" spans="1:51">
-      <c r="B7" s="96"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="98"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="115"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -5755,9 +5755,9 @@
       <c r="AY7"/>
     </row>
     <row r="8" spans="1:51">
-      <c r="B8" s="99"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="101"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="118"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
@@ -5774,38 +5774,38 @@
       <c r="AX9"/>
       <c r="AY9"/>
     </row>
-    <row r="10" spans="1:51" ht="19.95" customHeight="1" thickBot="1">
-      <c r="B10" s="105" t="s">
+    <row r="10" spans="1:51" ht="20" customHeight="1" thickBot="1">
+      <c r="B10" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="F10" s="105" t="s">
+      <c r="C10" s="123"/>
+      <c r="D10" s="124"/>
+      <c r="F10" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="106"/>
-      <c r="M10" s="107"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="124"/>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
-      <c r="R10" s="108" t="s">
+      <c r="R10" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="S10" s="109"/>
-      <c r="U10" s="108" t="s">
+      <c r="S10" s="126"/>
+      <c r="U10" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="V10" s="110"/>
-      <c r="W10" s="109"/>
-      <c r="AT10" s="102" t="s">
+      <c r="V10" s="127"/>
+      <c r="W10" s="126"/>
+      <c r="AT10" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="AU10" s="103"/>
-      <c r="AV10" s="104"/>
+      <c r="AU10" s="120"/>
+      <c r="AV10" s="121"/>
       <c r="AW10"/>
       <c r="AX10"/>
       <c r="AY10"/>
@@ -5865,7 +5865,7 @@
       <c r="S12" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="U12" s="123" t="s">
+      <c r="U12" s="96" t="s">
         <v>21</v>
       </c>
       <c r="V12" s="82" t="s">
@@ -5962,7 +5962,7 @@
       <c r="R13" s="14"/>
       <c r="S13" s="14"/>
       <c r="T13" s="8"/>
-      <c r="U13" s="124"/>
+      <c r="U13" s="97"/>
       <c r="V13" s="14"/>
       <c r="W13" s="14"/>
       <c r="X13" s="49"/>
@@ -6041,7 +6041,7 @@
       <c r="R14" s="54"/>
       <c r="S14" s="55"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="125">
+      <c r="U14" s="98">
         <f t="shared" ref="U14" si="0">EXP(AR14)</f>
         <v>1235.1019924733239</v>
       </c>
@@ -6186,7 +6186,7 @@
       <c r="R15" s="31"/>
       <c r="S15" s="32"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="126">
+      <c r="U15" s="99">
         <f t="shared" ref="U15:U78" si="14">EXP(AR15)</f>
         <v>1229.20792078863</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>1547.681</v>
       </c>
       <c r="Y15" s="41">
-        <f t="shared" ref="Y14:Y45" si="16">(F15/30.99)/($I15/60.08+$L15/79.9+$H15/50.98+$N15/71.85+$G15/40.32+$K15/56.08+$F15/30.99+$J15/47.1+$M15/70.94)</f>
+        <f t="shared" ref="Y15:Y45" si="16">(F15/30.99)/($I15/60.08+$L15/79.9+$H15/50.98+$N15/71.85+$G15/40.32+$K15/56.08+$F15/30.99+$J15/47.1+$M15/70.94)</f>
         <v>3.0720651850065273E-2</v>
       </c>
       <c r="Z15" s="42">
@@ -6254,7 +6254,7 @@
         <v>-2.0749548529901776</v>
       </c>
       <c r="AO15" s="42">
-        <f t="shared" ref="AO14:AO45" si="20">(137778-91.666*W15+8.474*W15*LN(W15))/(8.31441*W15)+(-291*D15+351*ERF(D15))/W15</f>
+        <f t="shared" ref="AO15:AO45" si="20">(137778-91.666*W15+8.474*W15*LN(W15))/(8.31441*W15)+(-291*D15+351*ERF(D15))/W15</f>
         <v>7.1865220098775495</v>
       </c>
       <c r="AP15" s="42">
@@ -6332,7 +6332,7 @@
       <c r="R16" s="31"/>
       <c r="S16" s="32"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="126">
+      <c r="U16" s="99">
         <f t="shared" si="14"/>
         <v>1216.4101697424694</v>
       </c>
@@ -6478,7 +6478,7 @@
       <c r="R17" s="31"/>
       <c r="S17" s="32"/>
       <c r="T17" s="4"/>
-      <c r="U17" s="126">
+      <c r="U17" s="99">
         <f t="shared" si="14"/>
         <v>1209.6129990483128</v>
       </c>
@@ -6624,7 +6624,7 @@
       <c r="R18" s="31"/>
       <c r="S18" s="32"/>
       <c r="T18" s="4"/>
-      <c r="U18" s="126">
+      <c r="U18" s="99">
         <f t="shared" si="14"/>
         <v>1195.5841585939538</v>
       </c>
@@ -6770,7 +6770,7 @@
       <c r="R19" s="31"/>
       <c r="S19" s="32"/>
       <c r="T19" s="4"/>
-      <c r="U19" s="126">
+      <c r="U19" s="99">
         <f t="shared" si="14"/>
         <v>1189.9170333485426</v>
       </c>
@@ -6916,7 +6916,7 @@
       <c r="R20" s="31"/>
       <c r="S20" s="32"/>
       <c r="T20" s="4"/>
-      <c r="U20" s="126">
+      <c r="U20" s="99">
         <f t="shared" si="14"/>
         <v>1188.6467497385763</v>
       </c>
@@ -7062,7 +7062,7 @@
       <c r="R21" s="31"/>
       <c r="S21" s="32"/>
       <c r="T21" s="4"/>
-      <c r="U21" s="126">
+      <c r="U21" s="99">
         <f t="shared" si="14"/>
         <v>1175.988425509111</v>
       </c>
@@ -7208,7 +7208,7 @@
       <c r="R22" s="31"/>
       <c r="S22" s="32"/>
       <c r="T22" s="4"/>
-      <c r="U22" s="126">
+      <c r="U22" s="99">
         <f t="shared" si="14"/>
         <v>1168.7147711892515</v>
       </c>
@@ -7354,7 +7354,7 @@
       <c r="R23" s="31"/>
       <c r="S23" s="32"/>
       <c r="T23" s="4"/>
-      <c r="U23" s="126">
+      <c r="U23" s="99">
         <f t="shared" si="14"/>
         <v>1161.0542150208578</v>
       </c>
@@ -7500,7 +7500,7 @@
       <c r="R24" s="31"/>
       <c r="S24" s="32"/>
       <c r="T24" s="4"/>
-      <c r="U24" s="126">
+      <c r="U24" s="99">
         <f t="shared" si="14"/>
         <v>1143.8104385359104</v>
       </c>
@@ -7646,7 +7646,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="32"/>
       <c r="T25" s="4"/>
-      <c r="U25" s="126">
+      <c r="U25" s="99">
         <f t="shared" si="14"/>
         <v>1134.6214314976437</v>
       </c>
@@ -7792,7 +7792,7 @@
       <c r="R26" s="31"/>
       <c r="S26" s="32"/>
       <c r="T26" s="4"/>
-      <c r="U26" s="126">
+      <c r="U26" s="99">
         <f t="shared" si="14"/>
         <v>1114.180569555645</v>
       </c>
@@ -7938,7 +7938,7 @@
       <c r="R27" s="31"/>
       <c r="S27" s="32"/>
       <c r="T27" s="4"/>
-      <c r="U27" s="126">
+      <c r="U27" s="99">
         <f t="shared" si="14"/>
         <v>1103.1070624106806</v>
       </c>
@@ -8084,7 +8084,7 @@
       <c r="R28" s="31"/>
       <c r="S28" s="32"/>
       <c r="T28" s="4"/>
-      <c r="U28" s="126">
+      <c r="U28" s="99">
         <f t="shared" si="14"/>
         <v>1091.5203438220601</v>
       </c>
@@ -8230,7 +8230,7 @@
       <c r="R29" s="31"/>
       <c r="S29" s="32"/>
       <c r="T29" s="4"/>
-      <c r="U29" s="126">
+      <c r="U29" s="99">
         <f t="shared" si="14"/>
         <v>1098.9226668726558</v>
       </c>
@@ -8376,7 +8376,7 @@
       <c r="R30" s="31"/>
       <c r="S30" s="32"/>
       <c r="T30" s="4"/>
-      <c r="U30" s="126">
+      <c r="U30" s="99">
         <f t="shared" si="14"/>
         <v>1106.4028923045585</v>
       </c>
@@ -8522,7 +8522,7 @@
       <c r="R31" s="31"/>
       <c r="S31" s="32"/>
       <c r="T31" s="4"/>
-      <c r="U31" s="126">
+      <c r="U31" s="99">
         <f t="shared" si="14"/>
         <v>1121.3257858012309</v>
       </c>
@@ -8668,7 +8668,7 @@
       <c r="R32" s="31"/>
       <c r="S32" s="32"/>
       <c r="T32" s="4"/>
-      <c r="U32" s="126">
+      <c r="U32" s="99">
         <f t="shared" si="14"/>
         <v>1129.0393064050477</v>
       </c>
@@ -8814,7 +8814,7 @@
       <c r="R33" s="31"/>
       <c r="S33" s="32"/>
       <c r="T33" s="4"/>
-      <c r="U33" s="126">
+      <c r="U33" s="99">
         <f t="shared" si="14"/>
         <v>1136.879436601376</v>
       </c>
@@ -8960,7 +8960,7 @@
       <c r="R34" s="31"/>
       <c r="S34" s="32"/>
       <c r="T34" s="4"/>
-      <c r="U34" s="126">
+      <c r="U34" s="99">
         <f t="shared" si="14"/>
         <v>1152.9672642264013</v>
       </c>
@@ -9106,7 +9106,7 @@
       <c r="R35" s="31"/>
       <c r="S35" s="32"/>
       <c r="T35" s="4"/>
-      <c r="U35" s="126">
+      <c r="U35" s="99">
         <f t="shared" si="14"/>
         <v>1161.3625290931082</v>
       </c>
@@ -9252,7 +9252,7 @@
       <c r="R36" s="31"/>
       <c r="S36" s="32"/>
       <c r="T36" s="4"/>
-      <c r="U36" s="126">
+      <c r="U36" s="99">
         <f t="shared" si="14"/>
         <v>1178.5902008254723</v>
       </c>
@@ -9398,7 +9398,7 @@
       <c r="R37" s="31"/>
       <c r="S37" s="32"/>
       <c r="T37" s="4"/>
-      <c r="U37" s="126">
+      <c r="U37" s="99">
         <f t="shared" si="14"/>
         <v>1187.3210397631415</v>
       </c>
@@ -9544,7 +9544,7 @@
       <c r="R38" s="31"/>
       <c r="S38" s="32"/>
       <c r="T38" s="4"/>
-      <c r="U38" s="126">
+      <c r="U38" s="99">
         <f t="shared" si="14"/>
         <v>1196.2386668877798</v>
       </c>
@@ -9690,7 +9690,7 @@
       <c r="R39" s="31"/>
       <c r="S39" s="32"/>
       <c r="T39" s="4"/>
-      <c r="U39" s="126">
+      <c r="U39" s="99">
         <f t="shared" si="14"/>
         <v>1214.7267125521525</v>
       </c>
@@ -9836,7 +9836,7 @@
       <c r="R40" s="31"/>
       <c r="S40" s="32"/>
       <c r="T40" s="4"/>
-      <c r="U40" s="126">
+      <c r="U40" s="99">
         <f t="shared" si="14"/>
         <v>1224.1752312182043</v>
       </c>
@@ -9982,7 +9982,7 @@
       <c r="R41" s="31"/>
       <c r="S41" s="32"/>
       <c r="T41" s="4"/>
-      <c r="U41" s="126">
+      <c r="U41" s="99">
         <f t="shared" si="14"/>
         <v>1233.934797088262</v>
       </c>
@@ -10128,7 +10128,7 @@
       <c r="R42" s="31"/>
       <c r="S42" s="32"/>
       <c r="T42" s="4"/>
-      <c r="U42" s="126">
+      <c r="U42" s="99">
         <f t="shared" si="14"/>
         <v>1253.9747657042703</v>
       </c>
@@ -10274,7 +10274,7 @@
       <c r="R43" s="31"/>
       <c r="S43" s="32"/>
       <c r="T43" s="4"/>
-      <c r="U43" s="126">
+      <c r="U43" s="99">
         <f t="shared" si="14"/>
         <v>1264.4706393787981</v>
       </c>
@@ -10420,7 +10420,7 @@
       <c r="R44" s="31"/>
       <c r="S44" s="32"/>
       <c r="T44" s="4"/>
-      <c r="U44" s="126">
+      <c r="U44" s="99">
         <f t="shared" si="14"/>
         <v>1285.9805603211314</v>
       </c>
@@ -10566,7 +10566,7 @@
       <c r="R45" s="31"/>
       <c r="S45" s="32"/>
       <c r="T45" s="4"/>
-      <c r="U45" s="126">
+      <c r="U45" s="99">
         <f t="shared" si="14"/>
         <v>1296.918347102416</v>
       </c>
@@ -10712,7 +10712,7 @@
       <c r="R46" s="31"/>
       <c r="S46" s="32"/>
       <c r="T46" s="4"/>
-      <c r="U46" s="126">
+      <c r="U46" s="99">
         <f t="shared" si="14"/>
         <v>1307.9634042655034</v>
       </c>
@@ -10858,7 +10858,7 @@
       <c r="R47" s="31"/>
       <c r="S47" s="32"/>
       <c r="T47" s="4"/>
-      <c r="U47" s="126">
+      <c r="U47" s="99">
         <f t="shared" si="14"/>
         <v>1331.5535539921455</v>
       </c>
@@ -11004,7 +11004,7 @@
       <c r="R48" s="31"/>
       <c r="S48" s="32"/>
       <c r="T48" s="4"/>
-      <c r="U48" s="126">
+      <c r="U48" s="99">
         <f t="shared" si="14"/>
         <v>1343.9288744192818</v>
       </c>
@@ -11150,7 +11150,7 @@
       <c r="R49" s="31"/>
       <c r="S49" s="32"/>
       <c r="T49" s="4"/>
-      <c r="U49" s="126">
+      <c r="U49" s="99">
         <f t="shared" si="14"/>
         <v>1369.0801037081367</v>
       </c>
@@ -11296,7 +11296,7 @@
       <c r="R50" s="31"/>
       <c r="S50" s="32"/>
       <c r="T50" s="4"/>
-      <c r="U50" s="126">
+      <c r="U50" s="99">
         <f t="shared" si="14"/>
         <v>1381.9735910331253</v>
       </c>
@@ -11442,7 +11442,7 @@
       <c r="R51" s="31"/>
       <c r="S51" s="32"/>
       <c r="T51" s="4"/>
-      <c r="U51" s="126">
+      <c r="U51" s="99">
         <f t="shared" si="14"/>
         <v>1395.344969893187</v>
       </c>
@@ -11588,7 +11588,7 @@
       <c r="R52" s="31"/>
       <c r="S52" s="32"/>
       <c r="T52" s="4"/>
-      <c r="U52" s="126">
+      <c r="U52" s="99">
         <f t="shared" si="14"/>
         <v>1423.1143704192755</v>
       </c>
@@ -11734,7 +11734,7 @@
       <c r="R53" s="31"/>
       <c r="S53" s="32"/>
       <c r="T53" s="4"/>
-      <c r="U53" s="126">
+      <c r="U53" s="99">
         <f t="shared" si="14"/>
         <v>1437.4541201218924</v>
       </c>
@@ -11880,7 +11880,7 @@
       <c r="R54" s="31"/>
       <c r="S54" s="32"/>
       <c r="T54" s="4"/>
-      <c r="U54" s="126">
+      <c r="U54" s="99">
         <f t="shared" si="14"/>
         <v>1467.2861068535292</v>
       </c>
@@ -12026,7 +12026,7 @@
       <c r="R55" s="31"/>
       <c r="S55" s="32"/>
       <c r="T55" s="4"/>
-      <c r="U55" s="126">
+      <c r="U55" s="99">
         <f t="shared" si="14"/>
         <v>1482.5027688359412</v>
       </c>
@@ -12172,7 +12172,7 @@
       <c r="R56" s="31"/>
       <c r="S56" s="32"/>
       <c r="T56" s="4"/>
-      <c r="U56" s="126">
+      <c r="U56" s="99">
         <f t="shared" si="14"/>
         <v>1498.210117189826</v>
       </c>
@@ -12315,7 +12315,7 @@
       <c r="R57" s="31"/>
       <c r="S57" s="32"/>
       <c r="T57" s="4"/>
-      <c r="U57" s="126">
+      <c r="U57" s="99">
         <f t="shared" si="14"/>
         <v>1530.9862755258671</v>
       </c>
@@ -12458,7 +12458,7 @@
       <c r="R58" s="31"/>
       <c r="S58" s="32"/>
       <c r="T58" s="4"/>
-      <c r="U58" s="126">
+      <c r="U58" s="99">
         <f t="shared" si="14"/>
         <v>1547.6854521396258</v>
       </c>
@@ -12601,7 +12601,7 @@
       <c r="R59" s="31"/>
       <c r="S59" s="32"/>
       <c r="T59" s="4"/>
-      <c r="U59" s="126">
+      <c r="U59" s="99">
         <f t="shared" si="14"/>
         <v>1564.0483193823486</v>
       </c>
@@ -12744,7 +12744,7 @@
       <c r="R60" s="31"/>
       <c r="S60" s="32"/>
       <c r="T60"/>
-      <c r="U60" s="126">
+      <c r="U60" s="99">
         <f t="shared" si="14"/>
         <v>1600.0916235970533</v>
       </c>
@@ -12890,7 +12890,7 @@
       <c r="R61" s="31"/>
       <c r="S61" s="32"/>
       <c r="T61" s="4"/>
-      <c r="U61" s="126">
+      <c r="U61" s="99">
         <f t="shared" si="14"/>
         <v>1618.1501512405639</v>
       </c>
@@ -13033,7 +13033,7 @@
       <c r="R62" s="31"/>
       <c r="S62" s="32"/>
       <c r="T62" s="4"/>
-      <c r="U62" s="126">
+      <c r="U62" s="99">
         <f t="shared" si="14"/>
         <v>1654.6259755399249</v>
       </c>
@@ -13154,7 +13154,7 @@
       <c r="R63" s="31"/>
       <c r="S63" s="32"/>
       <c r="T63" s="4"/>
-      <c r="U63" s="126" t="e">
+      <c r="U63" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -13277,7 +13277,7 @@
       <c r="R64" s="31"/>
       <c r="S64" s="32"/>
       <c r="T64" s="4"/>
-      <c r="U64" s="126" t="e">
+      <c r="U64" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -13400,7 +13400,7 @@
       <c r="R65" s="31"/>
       <c r="S65" s="32"/>
       <c r="T65" s="4"/>
-      <c r="U65" s="126" t="e">
+      <c r="U65" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -13523,7 +13523,7 @@
       <c r="R66" s="31"/>
       <c r="S66" s="32"/>
       <c r="T66" s="4"/>
-      <c r="U66" s="126" t="e">
+      <c r="U66" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -13646,7 +13646,7 @@
       <c r="R67" s="31"/>
       <c r="S67" s="32"/>
       <c r="T67" s="4"/>
-      <c r="U67" s="126" t="e">
+      <c r="U67" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -13769,7 +13769,7 @@
       <c r="R68" s="31"/>
       <c r="S68" s="32"/>
       <c r="T68" s="4"/>
-      <c r="U68" s="126" t="e">
+      <c r="U68" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -13892,7 +13892,7 @@
       <c r="R69" s="31"/>
       <c r="S69" s="32"/>
       <c r="T69" s="4"/>
-      <c r="U69" s="126" t="e">
+      <c r="U69" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14015,7 +14015,7 @@
       <c r="R70" s="31"/>
       <c r="S70" s="32"/>
       <c r="T70" s="4"/>
-      <c r="U70" s="126" t="e">
+      <c r="U70" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14138,7 +14138,7 @@
       <c r="R71" s="31"/>
       <c r="S71" s="32"/>
       <c r="T71" s="4"/>
-      <c r="U71" s="126" t="e">
+      <c r="U71" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14261,7 +14261,7 @@
       <c r="R72" s="31"/>
       <c r="S72" s="32"/>
       <c r="T72" s="4"/>
-      <c r="U72" s="126" t="e">
+      <c r="U72" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14384,7 +14384,7 @@
       <c r="R73" s="31"/>
       <c r="S73" s="32"/>
       <c r="T73" s="4"/>
-      <c r="U73" s="126" t="e">
+      <c r="U73" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14507,7 +14507,7 @@
       <c r="R74" s="31"/>
       <c r="S74" s="32"/>
       <c r="T74" s="4"/>
-      <c r="U74" s="126" t="e">
+      <c r="U74" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14630,7 +14630,7 @@
       <c r="R75" s="31"/>
       <c r="S75" s="32"/>
       <c r="T75" s="4"/>
-      <c r="U75" s="126" t="e">
+      <c r="U75" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14753,7 +14753,7 @@
       <c r="R76" s="31"/>
       <c r="S76" s="32"/>
       <c r="T76" s="4"/>
-      <c r="U76" s="126" t="e">
+      <c r="U76" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14876,7 +14876,7 @@
       <c r="R77" s="31"/>
       <c r="S77" s="32"/>
       <c r="T77" s="4"/>
-      <c r="U77" s="126" t="e">
+      <c r="U77" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -14999,7 +14999,7 @@
       <c r="R78" s="31"/>
       <c r="S78" s="32"/>
       <c r="T78" s="4"/>
-      <c r="U78" s="126" t="e">
+      <c r="U78" s="99" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
@@ -15122,7 +15122,7 @@
       <c r="R79" s="31"/>
       <c r="S79" s="32"/>
       <c r="T79" s="4"/>
-      <c r="U79" s="126" t="e">
+      <c r="U79" s="99" t="e">
         <f t="shared" ref="U79:U142" si="59">EXP(AR79)</f>
         <v>#DIV/0!</v>
       </c>
@@ -15245,7 +15245,7 @@
       <c r="R80" s="31"/>
       <c r="S80" s="32"/>
       <c r="T80"/>
-      <c r="U80" s="126" t="e">
+      <c r="U80" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -15371,7 +15371,7 @@
       <c r="R81" s="31"/>
       <c r="S81" s="32"/>
       <c r="T81" s="4"/>
-      <c r="U81" s="126" t="e">
+      <c r="U81" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -15494,7 +15494,7 @@
       <c r="R82" s="31"/>
       <c r="S82" s="32"/>
       <c r="T82"/>
-      <c r="U82" s="126" t="e">
+      <c r="U82" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -15620,7 +15620,7 @@
       <c r="R83" s="31"/>
       <c r="S83" s="32"/>
       <c r="T83" s="4"/>
-      <c r="U83" s="126" t="e">
+      <c r="U83" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -15743,7 +15743,7 @@
       <c r="R84" s="31"/>
       <c r="S84" s="32"/>
       <c r="T84" s="4"/>
-      <c r="U84" s="126" t="e">
+      <c r="U84" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -15869,7 +15869,7 @@
       <c r="R85" s="31"/>
       <c r="S85" s="32"/>
       <c r="T85" s="4"/>
-      <c r="U85" s="126" t="e">
+      <c r="U85" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -15992,7 +15992,7 @@
       <c r="R86" s="31"/>
       <c r="S86" s="32"/>
       <c r="T86" s="4"/>
-      <c r="U86" s="126" t="e">
+      <c r="U86" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16115,7 +16115,7 @@
       <c r="R87" s="31"/>
       <c r="S87" s="32"/>
       <c r="T87" s="4"/>
-      <c r="U87" s="126" t="e">
+      <c r="U87" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16241,7 +16241,7 @@
       <c r="R88" s="31"/>
       <c r="S88" s="32"/>
       <c r="T88" s="4"/>
-      <c r="U88" s="126" t="e">
+      <c r="U88" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16364,7 +16364,7 @@
       <c r="R89" s="31"/>
       <c r="S89" s="32"/>
       <c r="T89" s="4"/>
-      <c r="U89" s="126" t="e">
+      <c r="U89" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16487,7 +16487,7 @@
       <c r="R90" s="31"/>
       <c r="S90" s="32"/>
       <c r="T90"/>
-      <c r="U90" s="126" t="e">
+      <c r="U90" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16613,7 +16613,7 @@
       <c r="R91" s="31"/>
       <c r="S91" s="32"/>
       <c r="T91"/>
-      <c r="U91" s="126" t="e">
+      <c r="U91" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16739,7 +16739,7 @@
       <c r="R92" s="31"/>
       <c r="S92" s="32"/>
       <c r="T92"/>
-      <c r="U92" s="126" t="e">
+      <c r="U92" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16865,7 +16865,7 @@
       <c r="R93" s="31"/>
       <c r="S93" s="32"/>
       <c r="T93"/>
-      <c r="U93" s="126" t="e">
+      <c r="U93" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -16991,7 +16991,7 @@
       <c r="R94" s="31"/>
       <c r="S94" s="32"/>
       <c r="T94"/>
-      <c r="U94" s="126" t="e">
+      <c r="U94" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17117,7 +17117,7 @@
       <c r="R95" s="31"/>
       <c r="S95" s="32"/>
       <c r="T95" s="4"/>
-      <c r="U95" s="126" t="e">
+      <c r="U95" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17240,7 +17240,7 @@
       <c r="R96" s="31"/>
       <c r="S96" s="32"/>
       <c r="T96" s="4"/>
-      <c r="U96" s="126" t="e">
+      <c r="U96" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17363,7 +17363,7 @@
       <c r="R97" s="31"/>
       <c r="S97" s="32"/>
       <c r="T97" s="4"/>
-      <c r="U97" s="126" t="e">
+      <c r="U97" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17486,7 +17486,7 @@
       <c r="R98" s="31"/>
       <c r="S98" s="32"/>
       <c r="T98"/>
-      <c r="U98" s="126" t="e">
+      <c r="U98" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17612,7 +17612,7 @@
       <c r="R99" s="31"/>
       <c r="S99" s="32"/>
       <c r="T99"/>
-      <c r="U99" s="126" t="e">
+      <c r="U99" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17738,7 +17738,7 @@
       <c r="R100" s="31"/>
       <c r="S100" s="32"/>
       <c r="T100"/>
-      <c r="U100" s="126" t="e">
+      <c r="U100" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17864,7 +17864,7 @@
       <c r="R101" s="31"/>
       <c r="S101" s="32"/>
       <c r="T101"/>
-      <c r="U101" s="126" t="e">
+      <c r="U101" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -17990,7 +17990,7 @@
       <c r="R102" s="31"/>
       <c r="S102" s="32"/>
       <c r="T102"/>
-      <c r="U102" s="126" t="e">
+      <c r="U102" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18116,7 +18116,7 @@
       <c r="R103" s="31"/>
       <c r="S103" s="32"/>
       <c r="T103"/>
-      <c r="U103" s="126" t="e">
+      <c r="U103" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18242,7 +18242,7 @@
       <c r="R104" s="31"/>
       <c r="S104" s="32"/>
       <c r="T104"/>
-      <c r="U104" s="126" t="e">
+      <c r="U104" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18368,7 +18368,7 @@
       <c r="R105" s="31"/>
       <c r="S105" s="32"/>
       <c r="T105"/>
-      <c r="U105" s="126" t="e">
+      <c r="U105" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18494,7 +18494,7 @@
       <c r="R106" s="31"/>
       <c r="S106" s="32"/>
       <c r="T106"/>
-      <c r="U106" s="126" t="e">
+      <c r="U106" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18620,7 +18620,7 @@
       <c r="R107" s="31"/>
       <c r="S107" s="32"/>
       <c r="T107"/>
-      <c r="U107" s="126" t="e">
+      <c r="U107" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18746,7 +18746,7 @@
       <c r="R108" s="31"/>
       <c r="S108" s="32"/>
       <c r="T108"/>
-      <c r="U108" s="126" t="e">
+      <c r="U108" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18872,7 +18872,7 @@
       <c r="R109" s="31"/>
       <c r="S109" s="32"/>
       <c r="T109"/>
-      <c r="U109" s="126" t="e">
+      <c r="U109" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -18998,7 +18998,7 @@
       <c r="R110" s="31"/>
       <c r="S110" s="32"/>
       <c r="T110"/>
-      <c r="U110" s="126" t="e">
+      <c r="U110" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19124,7 +19124,7 @@
       <c r="R111" s="31"/>
       <c r="S111" s="32"/>
       <c r="T111"/>
-      <c r="U111" s="126" t="e">
+      <c r="U111" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19250,7 +19250,7 @@
       <c r="R112" s="31"/>
       <c r="S112" s="32"/>
       <c r="T112"/>
-      <c r="U112" s="126" t="e">
+      <c r="U112" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19376,7 +19376,7 @@
       <c r="R113" s="31"/>
       <c r="S113" s="32"/>
       <c r="T113"/>
-      <c r="U113" s="126" t="e">
+      <c r="U113" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19502,7 +19502,7 @@
       <c r="R114" s="31"/>
       <c r="S114" s="32"/>
       <c r="T114"/>
-      <c r="U114" s="126" t="e">
+      <c r="U114" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19628,7 +19628,7 @@
       <c r="R115" s="31"/>
       <c r="S115" s="32"/>
       <c r="T115"/>
-      <c r="U115" s="126" t="e">
+      <c r="U115" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19754,7 +19754,7 @@
       <c r="R116" s="31"/>
       <c r="S116" s="32"/>
       <c r="T116"/>
-      <c r="U116" s="126" t="e">
+      <c r="U116" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -19880,7 +19880,7 @@
       <c r="R117" s="31"/>
       <c r="S117" s="32"/>
       <c r="T117"/>
-      <c r="U117" s="126" t="e">
+      <c r="U117" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20006,7 +20006,7 @@
       <c r="R118" s="31"/>
       <c r="S118" s="32"/>
       <c r="T118"/>
-      <c r="U118" s="126" t="e">
+      <c r="U118" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20132,7 +20132,7 @@
       <c r="R119" s="31"/>
       <c r="S119" s="32"/>
       <c r="T119"/>
-      <c r="U119" s="126" t="e">
+      <c r="U119" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20258,7 +20258,7 @@
       <c r="R120" s="31"/>
       <c r="S120" s="32"/>
       <c r="T120"/>
-      <c r="U120" s="126" t="e">
+      <c r="U120" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20384,7 +20384,7 @@
       <c r="R121" s="31"/>
       <c r="S121" s="32"/>
       <c r="T121"/>
-      <c r="U121" s="126" t="e">
+      <c r="U121" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20510,7 +20510,7 @@
       <c r="R122" s="31"/>
       <c r="S122" s="32"/>
       <c r="T122"/>
-      <c r="U122" s="126" t="e">
+      <c r="U122" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20636,7 +20636,7 @@
       <c r="R123" s="31"/>
       <c r="S123" s="32"/>
       <c r="T123"/>
-      <c r="U123" s="126" t="e">
+      <c r="U123" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20762,7 +20762,7 @@
       <c r="R124" s="31"/>
       <c r="S124" s="32"/>
       <c r="T124"/>
-      <c r="U124" s="126" t="e">
+      <c r="U124" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -20888,7 +20888,7 @@
       <c r="R125" s="31"/>
       <c r="S125" s="32"/>
       <c r="T125"/>
-      <c r="U125" s="126" t="e">
+      <c r="U125" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21014,7 +21014,7 @@
       <c r="R126" s="31"/>
       <c r="S126" s="32"/>
       <c r="T126"/>
-      <c r="U126" s="126" t="e">
+      <c r="U126" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21140,7 +21140,7 @@
       <c r="R127" s="31"/>
       <c r="S127" s="32"/>
       <c r="T127"/>
-      <c r="U127" s="126" t="e">
+      <c r="U127" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21266,7 +21266,7 @@
       <c r="R128" s="31"/>
       <c r="S128" s="32"/>
       <c r="T128"/>
-      <c r="U128" s="126" t="e">
+      <c r="U128" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21392,7 +21392,7 @@
       <c r="R129" s="31"/>
       <c r="S129" s="32"/>
       <c r="T129"/>
-      <c r="U129" s="126" t="e">
+      <c r="U129" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21518,7 +21518,7 @@
       <c r="R130" s="31"/>
       <c r="S130" s="32"/>
       <c r="T130"/>
-      <c r="U130" s="126" t="e">
+      <c r="U130" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21644,7 +21644,7 @@
       <c r="R131" s="31"/>
       <c r="S131" s="32"/>
       <c r="T131"/>
-      <c r="U131" s="126" t="e">
+      <c r="U131" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21770,7 +21770,7 @@
       <c r="R132" s="31"/>
       <c r="S132" s="32"/>
       <c r="T132"/>
-      <c r="U132" s="126" t="e">
+      <c r="U132" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -21896,7 +21896,7 @@
       <c r="R133" s="31"/>
       <c r="S133" s="32"/>
       <c r="T133"/>
-      <c r="U133" s="126" t="e">
+      <c r="U133" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22022,7 +22022,7 @@
       <c r="R134" s="31"/>
       <c r="S134" s="32"/>
       <c r="T134"/>
-      <c r="U134" s="126" t="e">
+      <c r="U134" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22148,7 +22148,7 @@
       <c r="R135" s="31"/>
       <c r="S135" s="32"/>
       <c r="T135"/>
-      <c r="U135" s="126" t="e">
+      <c r="U135" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22274,7 +22274,7 @@
       <c r="R136" s="31"/>
       <c r="S136" s="32"/>
       <c r="T136"/>
-      <c r="U136" s="126" t="e">
+      <c r="U136" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22400,7 +22400,7 @@
       <c r="R137" s="31"/>
       <c r="S137" s="32"/>
       <c r="T137"/>
-      <c r="U137" s="126" t="e">
+      <c r="U137" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22526,7 +22526,7 @@
       <c r="R138" s="31"/>
       <c r="S138" s="32"/>
       <c r="T138"/>
-      <c r="U138" s="126" t="e">
+      <c r="U138" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22652,7 +22652,7 @@
       <c r="R139" s="31"/>
       <c r="S139" s="32"/>
       <c r="T139"/>
-      <c r="U139" s="126" t="e">
+      <c r="U139" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22778,7 +22778,7 @@
       <c r="R140" s="31"/>
       <c r="S140" s="32"/>
       <c r="T140"/>
-      <c r="U140" s="126" t="e">
+      <c r="U140" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -22904,7 +22904,7 @@
       <c r="R141" s="31"/>
       <c r="S141" s="32"/>
       <c r="T141"/>
-      <c r="U141" s="126" t="e">
+      <c r="U141" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -23030,7 +23030,7 @@
       <c r="R142" s="31"/>
       <c r="S142" s="32"/>
       <c r="T142"/>
-      <c r="U142" s="126" t="e">
+      <c r="U142" s="99" t="e">
         <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
@@ -23156,7 +23156,7 @@
       <c r="R143" s="31"/>
       <c r="S143" s="32"/>
       <c r="T143"/>
-      <c r="U143" s="126" t="e">
+      <c r="U143" s="99" t="e">
         <f t="shared" ref="U143:U160" si="100">EXP(AR143)</f>
         <v>#DIV/0!</v>
       </c>
@@ -23282,7 +23282,7 @@
       <c r="R144" s="31"/>
       <c r="S144" s="32"/>
       <c r="T144"/>
-      <c r="U144" s="126" t="e">
+      <c r="U144" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -23408,7 +23408,7 @@
       <c r="R145" s="31"/>
       <c r="S145" s="32"/>
       <c r="T145"/>
-      <c r="U145" s="126" t="e">
+      <c r="U145" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -23534,7 +23534,7 @@
       <c r="R146" s="31"/>
       <c r="S146" s="32"/>
       <c r="T146"/>
-      <c r="U146" s="126" t="e">
+      <c r="U146" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -23660,7 +23660,7 @@
       <c r="R147" s="31"/>
       <c r="S147" s="32"/>
       <c r="T147"/>
-      <c r="U147" s="126" t="e">
+      <c r="U147" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -23786,7 +23786,7 @@
       <c r="R148" s="31"/>
       <c r="S148" s="32"/>
       <c r="T148"/>
-      <c r="U148" s="126" t="e">
+      <c r="U148" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -23912,7 +23912,7 @@
       <c r="R149" s="31"/>
       <c r="S149" s="32"/>
       <c r="T149"/>
-      <c r="U149" s="126" t="e">
+      <c r="U149" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24038,7 +24038,7 @@
       <c r="R150" s="31"/>
       <c r="S150" s="32"/>
       <c r="T150"/>
-      <c r="U150" s="126" t="e">
+      <c r="U150" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24164,7 +24164,7 @@
       <c r="R151" s="31"/>
       <c r="S151" s="32"/>
       <c r="T151"/>
-      <c r="U151" s="126" t="e">
+      <c r="U151" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24290,7 +24290,7 @@
       <c r="R152" s="31"/>
       <c r="S152" s="32"/>
       <c r="T152"/>
-      <c r="U152" s="126" t="e">
+      <c r="U152" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24416,7 +24416,7 @@
       <c r="R153" s="31"/>
       <c r="S153" s="32"/>
       <c r="T153"/>
-      <c r="U153" s="126" t="e">
+      <c r="U153" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24542,7 +24542,7 @@
       <c r="R154" s="31"/>
       <c r="S154" s="32"/>
       <c r="T154"/>
-      <c r="U154" s="126" t="e">
+      <c r="U154" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24668,7 +24668,7 @@
       <c r="R155" s="31"/>
       <c r="S155" s="32"/>
       <c r="T155"/>
-      <c r="U155" s="126" t="e">
+      <c r="U155" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24794,7 +24794,7 @@
       <c r="R156" s="31"/>
       <c r="S156" s="32"/>
       <c r="T156"/>
-      <c r="U156" s="126" t="e">
+      <c r="U156" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -24920,7 +24920,7 @@
       <c r="R157" s="31"/>
       <c r="S157" s="32"/>
       <c r="T157"/>
-      <c r="U157" s="126" t="e">
+      <c r="U157" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -25046,7 +25046,7 @@
       <c r="R158" s="31"/>
       <c r="S158" s="32"/>
       <c r="T158"/>
-      <c r="U158" s="126" t="e">
+      <c r="U158" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -25172,7 +25172,7 @@
       <c r="R159" s="31"/>
       <c r="S159" s="32"/>
       <c r="T159"/>
-      <c r="U159" s="126" t="e">
+      <c r="U159" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -25298,7 +25298,7 @@
       <c r="R160" s="31"/>
       <c r="S160" s="32"/>
       <c r="T160"/>
-      <c r="U160" s="126" t="e">
+      <c r="U160" s="99" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
@@ -25418,7 +25418,7 @@
       <c r="R161" s="33"/>
       <c r="S161" s="34"/>
       <c r="T161"/>
-      <c r="U161" s="126" t="e">
+      <c r="U161" s="99" t="e">
         <f t="shared" ref="U161:U207" si="107">EXP(AR161)</f>
         <v>#DIV/0!</v>
       </c>
@@ -25537,7 +25537,7 @@
       <c r="R162" s="33"/>
       <c r="S162" s="34"/>
       <c r="T162"/>
-      <c r="U162" s="126" t="e">
+      <c r="U162" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -25656,7 +25656,7 @@
       <c r="R163" s="33"/>
       <c r="S163" s="34"/>
       <c r="T163"/>
-      <c r="U163" s="126" t="e">
+      <c r="U163" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -25775,7 +25775,7 @@
       <c r="R164" s="33"/>
       <c r="S164" s="34"/>
       <c r="T164"/>
-      <c r="U164" s="126" t="e">
+      <c r="U164" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -25894,7 +25894,7 @@
       <c r="R165" s="33"/>
       <c r="S165" s="34"/>
       <c r="T165"/>
-      <c r="U165" s="126" t="e">
+      <c r="U165" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26013,7 +26013,7 @@
       <c r="R166" s="33"/>
       <c r="S166" s="34"/>
       <c r="T166"/>
-      <c r="U166" s="126" t="e">
+      <c r="U166" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26132,7 +26132,7 @@
       <c r="R167" s="33"/>
       <c r="S167" s="34"/>
       <c r="T167"/>
-      <c r="U167" s="126" t="e">
+      <c r="U167" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26251,7 +26251,7 @@
       <c r="R168" s="33"/>
       <c r="S168" s="34"/>
       <c r="T168"/>
-      <c r="U168" s="126" t="e">
+      <c r="U168" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26370,7 +26370,7 @@
       <c r="R169" s="33"/>
       <c r="S169" s="34"/>
       <c r="T169"/>
-      <c r="U169" s="126" t="e">
+      <c r="U169" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26489,7 +26489,7 @@
       <c r="R170" s="33"/>
       <c r="S170" s="34"/>
       <c r="T170"/>
-      <c r="U170" s="126" t="e">
+      <c r="U170" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26608,7 +26608,7 @@
       <c r="R171" s="33"/>
       <c r="S171" s="34"/>
       <c r="T171"/>
-      <c r="U171" s="126" t="e">
+      <c r="U171" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26727,7 +26727,7 @@
       <c r="R172" s="33"/>
       <c r="S172" s="34"/>
       <c r="T172"/>
-      <c r="U172" s="126" t="e">
+      <c r="U172" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26846,7 +26846,7 @@
       <c r="R173" s="33"/>
       <c r="S173" s="34"/>
       <c r="T173"/>
-      <c r="U173" s="126" t="e">
+      <c r="U173" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -26965,7 +26965,7 @@
       <c r="R174" s="33"/>
       <c r="S174" s="34"/>
       <c r="T174"/>
-      <c r="U174" s="126" t="e">
+      <c r="U174" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27084,7 +27084,7 @@
       <c r="R175" s="33"/>
       <c r="S175" s="34"/>
       <c r="T175"/>
-      <c r="U175" s="126" t="e">
+      <c r="U175" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27202,7 +27202,7 @@
       <c r="Q176" s="11"/>
       <c r="R176" s="33"/>
       <c r="S176" s="34"/>
-      <c r="U176" s="126" t="e">
+      <c r="U176" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27318,7 +27318,7 @@
       <c r="Q177" s="11"/>
       <c r="R177" s="33"/>
       <c r="S177" s="34"/>
-      <c r="U177" s="126" t="e">
+      <c r="U177" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27434,7 +27434,7 @@
       <c r="Q178" s="11"/>
       <c r="R178" s="33"/>
       <c r="S178" s="34"/>
-      <c r="U178" s="126" t="e">
+      <c r="U178" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27550,7 +27550,7 @@
       <c r="Q179" s="11"/>
       <c r="R179" s="33"/>
       <c r="S179" s="34"/>
-      <c r="U179" s="126" t="e">
+      <c r="U179" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27666,7 +27666,7 @@
       <c r="Q180" s="11"/>
       <c r="R180" s="33"/>
       <c r="S180" s="34"/>
-      <c r="U180" s="126" t="e">
+      <c r="U180" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27782,7 +27782,7 @@
       <c r="Q181" s="11"/>
       <c r="R181" s="33"/>
       <c r="S181" s="34"/>
-      <c r="U181" s="126" t="e">
+      <c r="U181" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -27898,7 +27898,7 @@
       <c r="Q182" s="11"/>
       <c r="R182" s="33"/>
       <c r="S182" s="34"/>
-      <c r="U182" s="126" t="e">
+      <c r="U182" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28014,7 +28014,7 @@
       <c r="Q183" s="11"/>
       <c r="R183" s="33"/>
       <c r="S183" s="34"/>
-      <c r="U183" s="126" t="e">
+      <c r="U183" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28131,7 +28131,7 @@
       <c r="R184" s="33"/>
       <c r="S184" s="34"/>
       <c r="T184"/>
-      <c r="U184" s="126" t="e">
+      <c r="U184" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28250,7 +28250,7 @@
       <c r="R185" s="33"/>
       <c r="S185" s="34"/>
       <c r="T185"/>
-      <c r="U185" s="126" t="e">
+      <c r="U185" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28369,7 +28369,7 @@
       <c r="R186" s="33"/>
       <c r="S186" s="34"/>
       <c r="T186"/>
-      <c r="U186" s="126" t="e">
+      <c r="U186" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28488,7 +28488,7 @@
       <c r="R187" s="33"/>
       <c r="S187" s="34"/>
       <c r="T187"/>
-      <c r="U187" s="126" t="e">
+      <c r="U187" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28607,7 +28607,7 @@
       <c r="R188" s="33"/>
       <c r="S188" s="34"/>
       <c r="T188"/>
-      <c r="U188" s="126" t="e">
+      <c r="U188" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28726,7 +28726,7 @@
       <c r="R189" s="33"/>
       <c r="S189" s="34"/>
       <c r="T189"/>
-      <c r="U189" s="126" t="e">
+      <c r="U189" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28845,7 +28845,7 @@
       <c r="R190" s="33"/>
       <c r="S190" s="34"/>
       <c r="T190"/>
-      <c r="U190" s="126" t="e">
+      <c r="U190" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -28964,7 +28964,7 @@
       <c r="R191" s="33"/>
       <c r="S191" s="34"/>
       <c r="T191"/>
-      <c r="U191" s="126" t="e">
+      <c r="U191" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29083,7 +29083,7 @@
       <c r="R192" s="33"/>
       <c r="S192" s="34"/>
       <c r="T192"/>
-      <c r="U192" s="126" t="e">
+      <c r="U192" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29202,7 +29202,7 @@
       <c r="R193" s="33"/>
       <c r="S193" s="34"/>
       <c r="T193"/>
-      <c r="U193" s="126" t="e">
+      <c r="U193" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29320,7 +29320,7 @@
       <c r="Q194" s="11"/>
       <c r="R194" s="33"/>
       <c r="S194" s="34"/>
-      <c r="U194" s="126" t="e">
+      <c r="U194" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29435,7 +29435,7 @@
       <c r="Q195" s="11"/>
       <c r="R195" s="33"/>
       <c r="S195" s="34"/>
-      <c r="U195" s="126" t="e">
+      <c r="U195" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29550,7 +29550,7 @@
       <c r="Q196" s="11"/>
       <c r="R196" s="33"/>
       <c r="S196" s="34"/>
-      <c r="U196" s="126" t="e">
+      <c r="U196" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29665,7 +29665,7 @@
       <c r="Q197" s="11"/>
       <c r="R197" s="33"/>
       <c r="S197" s="34"/>
-      <c r="U197" s="126" t="e">
+      <c r="U197" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29780,7 +29780,7 @@
       <c r="Q198" s="11"/>
       <c r="R198" s="33"/>
       <c r="S198" s="34"/>
-      <c r="U198" s="126" t="e">
+      <c r="U198" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -29895,7 +29895,7 @@
       <c r="Q199" s="11"/>
       <c r="R199" s="33"/>
       <c r="S199" s="34"/>
-      <c r="U199" s="126" t="e">
+      <c r="U199" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30010,7 +30010,7 @@
       <c r="Q200" s="11"/>
       <c r="R200" s="33"/>
       <c r="S200" s="34"/>
-      <c r="U200" s="126" t="e">
+      <c r="U200" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30125,7 +30125,7 @@
       <c r="Q201" s="11"/>
       <c r="R201" s="33"/>
       <c r="S201" s="34"/>
-      <c r="U201" s="126" t="e">
+      <c r="U201" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30240,7 +30240,7 @@
       <c r="Q202" s="11"/>
       <c r="R202" s="33"/>
       <c r="S202" s="34"/>
-      <c r="U202" s="126" t="e">
+      <c r="U202" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30355,7 +30355,7 @@
       <c r="Q203" s="11"/>
       <c r="R203" s="33"/>
       <c r="S203" s="34"/>
-      <c r="U203" s="126" t="e">
+      <c r="U203" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30470,7 +30470,7 @@
       <c r="Q204" s="11"/>
       <c r="R204" s="33"/>
       <c r="S204" s="34"/>
-      <c r="U204" s="126" t="e">
+      <c r="U204" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30585,7 +30585,7 @@
       <c r="Q205" s="11"/>
       <c r="R205" s="33"/>
       <c r="S205" s="34"/>
-      <c r="U205" s="126" t="e">
+      <c r="U205" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30700,7 +30700,7 @@
       <c r="Q206" s="11"/>
       <c r="R206" s="33"/>
       <c r="S206" s="34"/>
-      <c r="U206" s="126" t="e">
+      <c r="U206" s="99" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30815,7 +30815,7 @@
       <c r="Q207" s="11"/>
       <c r="R207" s="35"/>
       <c r="S207" s="36"/>
-      <c r="U207" s="127" t="e">
+      <c r="U207" s="100" t="e">
         <f t="shared" si="107"/>
         <v>#DIV/0!</v>
       </c>
@@ -30925,7 +30925,7 @@
     <mergeCell ref="F10:M10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -30938,13 +30938,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF693-E754-4267-9E60-71E76129F09F}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.2" thickBot="1">
+    <row r="1" spans="1:18" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -31000,41 +31000,41 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="16.2" thickTop="1">
+    <row r="2" spans="1:18" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="111">
+      <c r="B2" s="84">
         <v>1.6941999999999999</v>
       </c>
-      <c r="C2" s="111">
+      <c r="C2" s="84">
         <v>10.8271</v>
       </c>
-      <c r="D2" s="111">
+      <c r="D2" s="84">
         <v>13.7783</v>
       </c>
-      <c r="E2" s="111">
+      <c r="E2" s="84">
         <v>49.862900000000003</v>
       </c>
-      <c r="F2" s="111">
+      <c r="F2" s="84">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="G2" s="111">
+      <c r="G2" s="84">
         <v>13.694800000000001</v>
       </c>
-      <c r="H2" s="111">
+      <c r="H2" s="84">
         <v>0.8165</v>
       </c>
-      <c r="I2" s="112">
+      <c r="I2" s="85">
         <v>0.1633</v>
       </c>
-      <c r="J2" s="111">
+      <c r="J2" s="84">
         <v>8.2349499000000002</v>
       </c>
-      <c r="K2" s="113">
+      <c r="K2" s="86">
         <v>204.1</v>
       </c>
-      <c r="L2" s="114">
+      <c r="L2" s="87">
         <v>91.9</v>
       </c>
       <c r="M2">
@@ -31061,37 +31061,37 @@
       <c r="A3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="111">
+      <c r="B3" s="84">
         <v>1.7097</v>
       </c>
-      <c r="C3" s="111">
+      <c r="C3" s="84">
         <v>10.753500000000001</v>
       </c>
-      <c r="D3" s="111">
+      <c r="D3" s="84">
         <v>13.8855</v>
       </c>
-      <c r="E3" s="111">
+      <c r="E3" s="84">
         <v>49.826799999999999</v>
       </c>
-      <c r="F3" s="111">
+      <c r="F3" s="84">
         <v>7.22E-2</v>
       </c>
-      <c r="G3" s="111">
+      <c r="G3" s="84">
         <v>13.6168</v>
       </c>
-      <c r="H3" s="111">
+      <c r="H3" s="84">
         <v>0.82199999999999995</v>
       </c>
-      <c r="I3" s="115">
+      <c r="I3" s="88">
         <v>0.16489999999999999</v>
       </c>
-      <c r="J3" s="111">
+      <c r="J3" s="84">
         <v>8.2842973999999998</v>
       </c>
-      <c r="K3" s="116">
+      <c r="K3" s="89">
         <v>200.8</v>
       </c>
-      <c r="L3" s="117">
+      <c r="L3" s="90">
         <v>92.6</v>
       </c>
       <c r="M3">
@@ -31118,37 +31118,37 @@
       <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="111">
+      <c r="B4" s="84">
         <v>1.7415</v>
       </c>
-      <c r="C4" s="111">
+      <c r="C4" s="84">
         <v>10.5983</v>
       </c>
-      <c r="D4" s="111">
+      <c r="D4" s="84">
         <v>14.1061</v>
       </c>
-      <c r="E4" s="111">
+      <c r="E4" s="84">
         <v>49.752400000000002</v>
       </c>
-      <c r="F4" s="111">
+      <c r="F4" s="84">
         <v>7.3599999999999999E-2</v>
       </c>
-      <c r="G4" s="111">
+      <c r="G4" s="84">
         <v>13.461</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="84">
         <v>0.83320000000000005</v>
       </c>
-      <c r="I4" s="115">
+      <c r="I4" s="88">
         <v>0.16830000000000001</v>
       </c>
-      <c r="J4" s="111">
+      <c r="J4" s="84">
         <v>8.3846924000000005</v>
       </c>
-      <c r="K4" s="116">
+      <c r="K4" s="89">
         <v>194.4</v>
       </c>
-      <c r="L4" s="117">
+      <c r="L4" s="90">
         <v>94.1</v>
       </c>
       <c r="M4">
@@ -31175,37 +31175,37 @@
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="111">
+      <c r="B5" s="84">
         <v>1.7579</v>
       </c>
-      <c r="C5" s="111">
+      <c r="C5" s="84">
         <v>10.5167</v>
       </c>
-      <c r="D5" s="111">
+      <c r="D5" s="84">
         <v>14.2195</v>
       </c>
-      <c r="E5" s="111">
+      <c r="E5" s="84">
         <v>49.714100000000002</v>
       </c>
-      <c r="F5" s="111">
+      <c r="F5" s="84">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="G5" s="111">
+      <c r="G5" s="84">
         <v>13.3834</v>
       </c>
-      <c r="H5" s="111">
+      <c r="H5" s="84">
         <v>0.83899999999999997</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5" s="88">
         <v>0.1701</v>
       </c>
-      <c r="J5" s="111">
+      <c r="J5" s="84">
         <v>8.4355499999999992</v>
       </c>
-      <c r="K5" s="116">
+      <c r="K5" s="89">
         <v>191.2</v>
       </c>
-      <c r="L5" s="117">
+      <c r="L5" s="90">
         <v>94.9</v>
       </c>
       <c r="M5">
@@ -31232,37 +31232,37 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="111">
+      <c r="B6" s="84">
         <v>1.7914000000000001</v>
       </c>
-      <c r="C6" s="111">
+      <c r="C6" s="84">
         <v>10.3467</v>
       </c>
-      <c r="D6" s="111">
+      <c r="D6" s="84">
         <v>14.450200000000001</v>
       </c>
-      <c r="E6" s="111">
+      <c r="E6" s="84">
         <v>49.636000000000003</v>
       </c>
-      <c r="F6" s="111">
+      <c r="F6" s="84">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="G6" s="111">
+      <c r="G6" s="84">
         <v>13.2303</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="84">
         <v>0.8508</v>
       </c>
-      <c r="I6" s="115">
+      <c r="I6" s="88">
         <v>0.17369999999999999</v>
       </c>
-      <c r="J6" s="111">
+      <c r="J6" s="84">
         <v>8.5381651999999999</v>
       </c>
-      <c r="K6" s="116">
+      <c r="K6" s="89">
         <v>184.9</v>
       </c>
-      <c r="L6" s="117">
+      <c r="L6" s="90">
         <v>96.5</v>
       </c>
       <c r="M6">
@@ -31289,37 +31289,37 @@
       <c r="A7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="111">
+      <c r="B7" s="84">
         <v>1.8050999999999999</v>
       </c>
-      <c r="C7" s="111">
+      <c r="C7" s="84">
         <v>10.273</v>
       </c>
-      <c r="D7" s="111">
+      <c r="D7" s="84">
         <v>14.544600000000001</v>
       </c>
-      <c r="E7" s="111">
+      <c r="E7" s="84">
         <v>49.6053</v>
       </c>
-      <c r="F7" s="111">
+      <c r="F7" s="84">
         <v>7.6600000000000001E-2</v>
       </c>
-      <c r="G7" s="111">
+      <c r="G7" s="84">
         <v>13.1717</v>
       </c>
-      <c r="H7" s="111">
+      <c r="H7" s="84">
         <v>0.85560000000000003</v>
       </c>
-      <c r="I7" s="115">
+      <c r="I7" s="88">
         <v>0.17519999999999999</v>
       </c>
-      <c r="J7" s="111">
+      <c r="J7" s="84">
         <v>8.5787834000000007</v>
       </c>
-      <c r="K7" s="116">
+      <c r="K7" s="89">
         <v>182.2</v>
       </c>
-      <c r="L7" s="117">
+      <c r="L7" s="90">
         <v>97.1</v>
       </c>
       <c r="M7">
@@ -31346,37 +31346,37 @@
       <c r="A8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="111">
+      <c r="B8" s="84">
         <v>1.8088</v>
       </c>
-      <c r="C8" s="111">
+      <c r="C8" s="84">
         <v>10.2425</v>
       </c>
-      <c r="D8" s="111">
+      <c r="D8" s="84">
         <v>14.570399999999999</v>
       </c>
-      <c r="E8" s="111">
+      <c r="E8" s="84">
         <v>49.6021</v>
       </c>
-      <c r="F8" s="111">
+      <c r="F8" s="84">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="G8" s="111">
+      <c r="G8" s="84">
         <v>13.164300000000001</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="84">
         <v>0.8569</v>
       </c>
-      <c r="I8" s="115">
+      <c r="I8" s="88">
         <v>0.17560000000000001</v>
       </c>
-      <c r="J8" s="111">
+      <c r="J8" s="84">
         <v>8.5867430000000002</v>
       </c>
-      <c r="K8" s="116">
+      <c r="K8" s="89">
         <v>180.9</v>
       </c>
-      <c r="L8" s="117">
+      <c r="L8" s="90">
         <v>97.3</v>
       </c>
       <c r="M8">
@@ -31403,37 +31403,37 @@
       <c r="A9" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="111">
+      <c r="B9" s="84">
         <v>1.8451</v>
       </c>
-      <c r="C9" s="111">
+      <c r="C9" s="84">
         <v>9.9426000000000005</v>
       </c>
-      <c r="D9" s="111">
+      <c r="D9" s="84">
         <v>14.827199999999999</v>
       </c>
-      <c r="E9" s="111">
+      <c r="E9" s="84">
         <v>49.568800000000003</v>
       </c>
-      <c r="F9" s="111">
+      <c r="F9" s="84">
         <v>7.85E-2</v>
       </c>
-      <c r="G9" s="111">
+      <c r="G9" s="84">
         <v>13.087899999999999</v>
       </c>
-      <c r="H9" s="111">
+      <c r="H9" s="84">
         <v>0.87050000000000005</v>
       </c>
-      <c r="I9" s="115">
+      <c r="I9" s="88">
         <v>0.17949999999999999</v>
       </c>
-      <c r="J9" s="111">
+      <c r="J9" s="84">
         <v>8.6661591999999992</v>
       </c>
-      <c r="K9" s="116">
+      <c r="K9" s="89">
         <v>168.6</v>
       </c>
-      <c r="L9" s="117">
+      <c r="L9" s="90">
         <v>99</v>
       </c>
       <c r="M9">
@@ -31460,37 +31460,37 @@
       <c r="A10" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="111">
+      <c r="B10" s="84">
         <v>1.8635999999999999</v>
       </c>
-      <c r="C10" s="111">
+      <c r="C10" s="84">
         <v>9.7927999999999997</v>
       </c>
-      <c r="D10" s="111">
+      <c r="D10" s="84">
         <v>14.9575</v>
       </c>
-      <c r="E10" s="111">
+      <c r="E10" s="84">
         <v>49.550899999999999</v>
       </c>
-      <c r="F10" s="111">
+      <c r="F10" s="84">
         <v>7.9399999999999998E-2</v>
       </c>
-      <c r="G10" s="111">
+      <c r="G10" s="84">
         <v>13.047800000000001</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="84">
         <v>0.87729999999999997</v>
       </c>
-      <c r="I10" s="115">
+      <c r="I10" s="88">
         <v>0.18140000000000001</v>
       </c>
-      <c r="J10" s="111">
+      <c r="J10" s="84">
         <v>8.7060975999999997</v>
       </c>
-      <c r="K10" s="116">
+      <c r="K10" s="89">
         <v>162.80000000000001</v>
       </c>
-      <c r="L10" s="117">
+      <c r="L10" s="90">
         <v>99.9</v>
       </c>
       <c r="M10">
@@ -31517,37 +31517,37 @@
       <c r="A11" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="111">
+      <c r="B11" s="84">
         <v>1.8826000000000001</v>
       </c>
-      <c r="C11" s="111">
+      <c r="C11" s="84">
         <v>9.6371000000000002</v>
       </c>
-      <c r="D11" s="111">
+      <c r="D11" s="84">
         <v>15.0913</v>
       </c>
-      <c r="E11" s="111">
+      <c r="E11" s="84">
         <v>49.533799999999999</v>
       </c>
-      <c r="F11" s="111">
+      <c r="F11" s="84">
         <v>8.0299999999999996E-2</v>
       </c>
-      <c r="G11" s="111">
+      <c r="G11" s="84">
         <v>13.008699999999999</v>
       </c>
-      <c r="H11" s="111">
+      <c r="H11" s="84">
         <v>0.88429999999999997</v>
       </c>
-      <c r="I11" s="115">
+      <c r="I11" s="88">
         <v>0.1835</v>
       </c>
-      <c r="J11" s="111">
+      <c r="J11" s="84">
         <v>8.7456461000000001</v>
       </c>
-      <c r="K11" s="116">
+      <c r="K11" s="89">
         <v>156.9</v>
       </c>
-      <c r="L11" s="117">
+      <c r="L11" s="90">
         <v>100.8</v>
       </c>
       <c r="M11">
@@ -31574,37 +31574,37 @@
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="111">
+      <c r="B12" s="84">
         <v>1.9216</v>
       </c>
-      <c r="C12" s="111">
+      <c r="C12" s="84">
         <v>9.3247999999999998</v>
       </c>
-      <c r="D12" s="111">
+      <c r="D12" s="84">
         <v>15.363799999999999</v>
       </c>
-      <c r="E12" s="111">
+      <c r="E12" s="84">
         <v>49.496699999999997</v>
       </c>
-      <c r="F12" s="111">
+      <c r="F12" s="84">
         <v>8.2100000000000006E-2</v>
       </c>
-      <c r="G12" s="111">
+      <c r="G12" s="84">
         <v>12.9262</v>
       </c>
-      <c r="H12" s="111">
+      <c r="H12" s="84">
         <v>0.89859999999999995</v>
       </c>
-      <c r="I12" s="115">
+      <c r="I12" s="88">
         <v>0.18770000000000001</v>
       </c>
-      <c r="J12" s="111">
+      <c r="J12" s="84">
         <v>8.8256835000000002</v>
       </c>
-      <c r="K12" s="116">
+      <c r="K12" s="89">
         <v>145.9</v>
       </c>
-      <c r="L12" s="117">
+      <c r="L12" s="90">
         <v>102.7</v>
       </c>
       <c r="M12">
@@ -31631,37 +31631,37 @@
       <c r="A13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="111">
+      <c r="B13" s="84">
         <v>1.9417</v>
       </c>
-      <c r="C13" s="111">
+      <c r="C13" s="84">
         <v>9.1672999999999991</v>
       </c>
-      <c r="D13" s="111">
+      <c r="D13" s="84">
         <v>15.5038</v>
       </c>
-      <c r="E13" s="111">
+      <c r="E13" s="84">
         <v>49.476500000000001</v>
       </c>
-      <c r="F13" s="111">
+      <c r="F13" s="84">
         <v>8.3099999999999993E-2</v>
       </c>
-      <c r="G13" s="111">
+      <c r="G13" s="84">
         <v>12.882199999999999</v>
       </c>
-      <c r="H13" s="111">
+      <c r="H13" s="84">
         <v>0.90600000000000003</v>
       </c>
-      <c r="I13" s="115">
+      <c r="I13" s="88">
         <v>0.18990000000000001</v>
       </c>
-      <c r="J13" s="111">
+      <c r="J13" s="84">
         <v>8.8664723999999993</v>
       </c>
-      <c r="K13" s="116">
+      <c r="K13" s="89">
         <v>140.6</v>
       </c>
-      <c r="L13" s="117">
+      <c r="L13" s="90">
         <v>103.6</v>
       </c>
       <c r="M13">
@@ -31688,37 +31688,37 @@
       <c r="A14" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="111">
+      <c r="B14" s="84">
         <v>1.9830000000000001</v>
       </c>
-      <c r="C14" s="111">
+      <c r="C14" s="84">
         <v>8.8453999999999997</v>
       </c>
-      <c r="D14" s="111">
+      <c r="D14" s="84">
         <v>15.7895</v>
       </c>
-      <c r="E14" s="111">
+      <c r="E14" s="84">
         <v>49.435899999999997</v>
       </c>
-      <c r="F14" s="111">
+      <c r="F14" s="84">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G14" s="111">
+      <c r="G14" s="84">
         <v>12.7943</v>
       </c>
-      <c r="H14" s="111">
+      <c r="H14" s="84">
         <v>0.92090000000000005</v>
       </c>
-      <c r="I14" s="115">
+      <c r="I14" s="88">
         <v>0.19439999999999999</v>
       </c>
-      <c r="J14" s="111">
+      <c r="J14" s="84">
         <v>8.9468209000000005</v>
       </c>
-      <c r="K14" s="116">
+      <c r="K14" s="89">
         <v>130.5</v>
       </c>
-      <c r="L14" s="117">
+      <c r="L14" s="90">
         <v>105.6</v>
       </c>
       <c r="M14">
@@ -31745,37 +31745,37 @@
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="111">
+      <c r="B15" s="84">
         <v>2.0043000000000002</v>
       </c>
-      <c r="C15" s="111">
+      <c r="C15" s="84">
         <v>8.6828000000000003</v>
       </c>
-      <c r="D15" s="111">
+      <c r="D15" s="84">
         <v>15.9361</v>
       </c>
-      <c r="E15" s="111">
+      <c r="E15" s="84">
         <v>49.414000000000001</v>
       </c>
-      <c r="F15" s="111">
+      <c r="F15" s="84">
         <v>8.6099999999999996E-2</v>
       </c>
-      <c r="G15" s="111">
+      <c r="G15" s="84">
         <v>12.7478</v>
       </c>
-      <c r="H15" s="111">
+      <c r="H15" s="84">
         <v>0.92859999999999998</v>
       </c>
-      <c r="I15" s="115">
+      <c r="I15" s="88">
         <v>0.19670000000000001</v>
       </c>
-      <c r="J15" s="111">
+      <c r="J15" s="84">
         <v>8.9876602999999999</v>
       </c>
-      <c r="K15" s="116">
+      <c r="K15" s="89">
         <v>125.8</v>
       </c>
-      <c r="L15" s="117">
+      <c r="L15" s="90">
         <v>106.6</v>
       </c>
       <c r="M15">
@@ -31802,37 +31802,37 @@
       <c r="A16" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="111">
+      <c r="B16" s="84">
         <v>2.0259</v>
       </c>
-      <c r="C16" s="111">
+      <c r="C16" s="84">
         <v>8.5206999999999997</v>
       </c>
-      <c r="D16" s="111">
+      <c r="D16" s="84">
         <v>16.084099999999999</v>
       </c>
-      <c r="E16" s="111">
+      <c r="E16" s="84">
         <v>49.390900000000002</v>
       </c>
-      <c r="F16" s="111">
+      <c r="F16" s="84">
         <v>8.7099999999999997E-2</v>
       </c>
-      <c r="G16" s="111">
+      <c r="G16" s="84">
         <v>12.6997</v>
       </c>
-      <c r="H16" s="111">
+      <c r="H16" s="84">
         <v>0.93630000000000002</v>
       </c>
-      <c r="I16" s="115">
+      <c r="I16" s="88">
         <v>0.1991</v>
       </c>
-      <c r="J16" s="111">
+      <c r="J16" s="84">
         <v>9.0286299999999997</v>
       </c>
-      <c r="K16" s="116">
+      <c r="K16" s="89">
         <v>121.2</v>
       </c>
-      <c r="L16" s="117">
+      <c r="L16" s="90">
         <v>107.7</v>
       </c>
       <c r="M16">
@@ -31859,37 +31859,37 @@
       <c r="A17" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="111">
+      <c r="B17" s="84">
         <v>2.0345</v>
       </c>
-      <c r="C17" s="111">
+      <c r="C17" s="84">
         <v>8.4794999999999998</v>
       </c>
-      <c r="D17" s="111">
+      <c r="D17" s="84">
         <v>16.040500000000002</v>
       </c>
-      <c r="E17" s="111">
+      <c r="E17" s="84">
         <v>49.399099999999997</v>
       </c>
-      <c r="F17" s="111">
+      <c r="F17" s="84">
         <v>8.8200000000000001E-2</v>
       </c>
-      <c r="G17" s="111">
+      <c r="G17" s="84">
         <v>12.668699999999999</v>
       </c>
-      <c r="H17" s="111">
+      <c r="H17" s="84">
         <v>0.94650000000000001</v>
       </c>
-      <c r="I17" s="115">
+      <c r="I17" s="88">
         <v>0.2016</v>
       </c>
-      <c r="J17" s="111">
+      <c r="J17" s="84">
         <v>9.1016776000000004</v>
       </c>
-      <c r="K17" s="116">
+      <c r="K17" s="89">
         <v>118.9</v>
       </c>
-      <c r="L17" s="117">
+      <c r="L17" s="90">
         <v>108.8</v>
       </c>
       <c r="M17">
@@ -31916,37 +31916,37 @@
       <c r="A18" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="111">
+      <c r="B18" s="84">
         <v>2.0432999999999999</v>
       </c>
-      <c r="C18" s="111">
+      <c r="C18" s="84">
         <v>8.44</v>
       </c>
-      <c r="D18" s="111">
+      <c r="D18" s="84">
         <v>15.997199999999999</v>
       </c>
-      <c r="E18" s="111">
+      <c r="E18" s="84">
         <v>49.405700000000003</v>
       </c>
-      <c r="F18" s="111">
+      <c r="F18" s="84">
         <v>8.9300000000000004E-2</v>
       </c>
-      <c r="G18" s="111">
+      <c r="G18" s="84">
         <v>12.6348</v>
       </c>
-      <c r="H18" s="111">
+      <c r="H18" s="84">
         <v>0.95679999999999998</v>
       </c>
-      <c r="I18" s="115">
+      <c r="I18" s="88">
         <v>0.2041</v>
       </c>
-      <c r="J18" s="111">
+      <c r="J18" s="84">
         <v>9.1766050000000003</v>
       </c>
-      <c r="K18" s="116">
+      <c r="K18" s="89">
         <v>116.6</v>
       </c>
-      <c r="L18" s="117">
+      <c r="L18" s="90">
         <v>109.9</v>
       </c>
       <c r="M18">
@@ -31973,37 +31973,37 @@
       <c r="A19" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="111">
+      <c r="B19" s="84">
         <v>2.0611999999999999</v>
       </c>
-      <c r="C19" s="111">
+      <c r="C19" s="84">
         <v>8.3582999999999998</v>
       </c>
-      <c r="D19" s="111">
+      <c r="D19" s="84">
         <v>15.907</v>
       </c>
-      <c r="E19" s="111">
+      <c r="E19" s="84">
         <v>49.419699999999999</v>
       </c>
-      <c r="F19" s="111">
+      <c r="F19" s="84">
         <v>9.1600000000000001E-2</v>
       </c>
-      <c r="G19" s="111">
+      <c r="G19" s="84">
         <v>12.565899999999999</v>
       </c>
-      <c r="H19" s="111">
+      <c r="H19" s="84">
         <v>0.97829999999999995</v>
       </c>
-      <c r="I19" s="115">
+      <c r="I19" s="88">
         <v>0.2094</v>
       </c>
-      <c r="J19" s="111">
+      <c r="J19" s="84">
         <v>9.3305992</v>
       </c>
-      <c r="K19" s="116">
+      <c r="K19" s="89">
         <v>112.2</v>
       </c>
-      <c r="L19" s="117">
+      <c r="L19" s="90">
         <v>112.3</v>
       </c>
       <c r="M19">
@@ -32030,37 +32030,37 @@
       <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="111">
+      <c r="B20" s="84">
         <v>2.0705</v>
       </c>
-      <c r="C20" s="111">
+      <c r="C20" s="84">
         <v>8.3141999999999996</v>
       </c>
-      <c r="D20" s="111">
+      <c r="D20" s="84">
         <v>15.863099999999999</v>
       </c>
-      <c r="E20" s="111">
+      <c r="E20" s="84">
         <v>49.426600000000001</v>
       </c>
-      <c r="F20" s="111">
+      <c r="F20" s="84">
         <v>9.2799999999999994E-2</v>
       </c>
-      <c r="G20" s="111">
+      <c r="G20" s="84">
         <v>12.5304</v>
       </c>
-      <c r="H20" s="111">
+      <c r="H20" s="84">
         <v>0.98939999999999995</v>
       </c>
-      <c r="I20" s="115">
+      <c r="I20" s="88">
         <v>0.21210000000000001</v>
       </c>
-      <c r="J20" s="111">
+      <c r="J20" s="84">
         <v>9.4093660000000003</v>
       </c>
-      <c r="K20" s="116">
+      <c r="K20" s="89">
         <v>109.9</v>
       </c>
-      <c r="L20" s="117">
+      <c r="L20" s="90">
         <v>113.5</v>
       </c>
       <c r="M20">
@@ -32087,37 +32087,37 @@
       <c r="A21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="111">
+      <c r="B21" s="84">
         <v>2.0798000000000001</v>
       </c>
-      <c r="C21" s="111">
+      <c r="C21" s="84">
         <v>8.2716999999999992</v>
       </c>
-      <c r="D21" s="111">
+      <c r="D21" s="84">
         <v>15.815200000000001</v>
       </c>
-      <c r="E21" s="111">
+      <c r="E21" s="84">
         <v>49.433700000000002</v>
       </c>
-      <c r="F21" s="111">
+      <c r="F21" s="84">
         <v>9.4E-2</v>
       </c>
-      <c r="G21" s="111">
+      <c r="G21" s="84">
         <v>12.4939</v>
       </c>
-      <c r="H21" s="111">
+      <c r="H21" s="84">
         <v>1.0007999999999999</v>
       </c>
-      <c r="I21" s="115">
+      <c r="I21" s="88">
         <v>0.21490000000000001</v>
       </c>
-      <c r="J21" s="111">
+      <c r="J21" s="84">
         <v>9.4906822999999996</v>
       </c>
-      <c r="K21" s="116">
+      <c r="K21" s="89">
         <v>107.7</v>
       </c>
-      <c r="L21" s="117">
+      <c r="L21" s="90">
         <v>114.8</v>
       </c>
       <c r="M21">
@@ -32144,37 +32144,37 @@
       <c r="A22" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="118">
+      <c r="B22" s="91">
         <v>2.0989</v>
       </c>
-      <c r="C22" s="118">
+      <c r="C22" s="91">
         <v>8.1811000000000007</v>
       </c>
-      <c r="D22" s="118">
+      <c r="D22" s="91">
         <v>15.7204</v>
       </c>
-      <c r="E22" s="118">
+      <c r="E22" s="91">
         <v>49.4482</v>
       </c>
-      <c r="F22" s="118">
+      <c r="F22" s="91">
         <v>9.6500000000000002E-2</v>
       </c>
-      <c r="G22" s="118">
+      <c r="G22" s="91">
         <v>12.4194</v>
       </c>
-      <c r="H22" s="118">
+      <c r="H22" s="91">
         <v>1.0243</v>
       </c>
-      <c r="I22" s="119">
+      <c r="I22" s="92">
         <v>0.22070000000000001</v>
       </c>
-      <c r="J22" s="118">
+      <c r="J22" s="91">
         <v>9.6563745000000001</v>
       </c>
-      <c r="K22" s="120">
+      <c r="K22" s="93">
         <v>103.2</v>
       </c>
-      <c r="L22" s="121">
+      <c r="L22" s="94">
         <v>117.4</v>
       </c>
       <c r="M22">

</xml_diff>